<commit_message>
added chisel config files for adaptive tests
</commit_message>
<xml_diff>
--- a/builds.xlsx
+++ b/builds.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Bit width</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>build-dc-2014-05-05_22-51</t>
+  </si>
+  <si>
+    <t>Area AdaptiveDecoder</t>
+  </si>
+  <si>
+    <t>Area Matrix</t>
+  </si>
+  <si>
+    <t>Effective Area</t>
   </si>
 </sst>
 </file>
@@ -368,21 +377,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -393,19 +403,28 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>24</v>
       </c>
@@ -415,21 +434,21 @@
       <c r="D2">
         <v>0.49099999999999999</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>57.8</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>100</v>
       </c>
-      <c r="G2">
-        <f>1000/F2</f>
+      <c r="J2">
+        <f>1000/I2</f>
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -437,19 +456,29 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0.41599999999999998</v>
+        <v>0.47199999999999998</v>
       </c>
       <c r="E3">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="G3">
+        <f>D3+1*(E3+F3)</f>
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="H3">
         <v>51.4</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>28.5</v>
       </c>
-      <c r="G3">
-        <f>1000/F3</f>
+      <c r="J3">
+        <f>1000/I3</f>
         <v>35.087719298245617</v>
       </c>
-      <c r="I3" t="s">
+      <c r="L3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
last build data updated
</commit_message>
<xml_diff>
--- a/builds.xlsx
+++ b/builds.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Bit width</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>build-dc-2014-05-05_23-46</t>
+  </si>
+  <si>
+    <t>Simon's account</t>
   </si>
 </sst>
 </file>
@@ -380,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,6 +522,40 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="E5">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.16900000000000001</v>
+      </c>
+      <c r="G5">
+        <f>D5</f>
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="H5">
+        <v>55.5</v>
+      </c>
+      <c r="I5">
+        <v>14</v>
+      </c>
+      <c r="J5">
+        <f>1000/I5</f>
+        <v>71.428571428571431</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>